<commit_message>
adapted pie charts, more PhiPT calcs, more perenniality calcs & KON graph
</commit_message>
<xml_diff>
--- a/Structure_ClusterAssignMLGs.xlsx
+++ b/Structure_ClusterAssignMLGs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wslch365-my.sharepoint.com/personal/lia_baumann_wsl_ch/Documents/R/truffles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{BE708B57-0892-3643-8382-6397C0CF8B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EEB02C3-EB12-49CD-B099-046CF540ACFB}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{BE708B57-0892-3643-8382-6397C0CF8B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A24BCB79-889D-47BF-A7E0-89D39F1B76C9}"/>
   <bookViews>
-    <workbookView xWindow="56265" yWindow="4380" windowWidth="21465" windowHeight="12705" activeTab="1" xr2:uid="{8B2E2298-6B14-B241-BB17-062C1F5FB235}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8B2E2298-6B14-B241-BB17-062C1F5FB235}"/>
   </bookViews>
   <sheets>
     <sheet name="ClumppIndFileMLGref" sheetId="1" r:id="rId1"/>
@@ -3808,9 +3808,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3CECD6D-642C-7749-BC0C-99E9BDDE3D35}">
   <dimension ref="A1:AB468"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" activeCellId="6" sqref="M1:M1048576 E1:E1048576 F1:F1048576 G1:G1048576 H1:H1048576 I1:I1048576 J1:J1048576"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2:M468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -44078,7 +44078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF226374-6849-45DA-821D-62BB3A671EA6}">
   <dimension ref="A1:G468"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>